<commit_message>
gpu benchmark comparison spreadsheet
</commit_message>
<xml_diff>
--- a/sheets/gpu-comparisons.xlsx
+++ b/sheets/gpu-comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terry\source\repos\tensorflow2_notebooks\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EC5BD2-B2D0-41C4-9AC5-BFB4CFCFC2E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9EDBA6-DD12-4A9A-BE1C-8A935A146B3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1896" yWindow="2064" windowWidth="23040" windowHeight="12204" xr2:uid="{88C7784B-2542-44DA-8D7C-FF5E767CAADD}"/>
+    <workbookView xWindow="7788" yWindow="-60" windowWidth="23040" windowHeight="12204" xr2:uid="{88C7784B-2542-44DA-8D7C-FF5E767CAADD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>RTX A6000</t>
   </si>
   <si>
-    <t>RTX A100</t>
-  </si>
-  <si>
     <t>https://www.evolution.ai/post/benchmarking-deep-learning-workloads-with-tensorflow-on-the-nvidia-geforce-rtx-3090?ref=brianlovin.com</t>
   </si>
   <si>
@@ -91,13 +88,16 @@
   </si>
   <si>
     <t>Note: Models may be much bigger than InceptionV4.</t>
+  </si>
+  <si>
+    <t>A100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +130,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,13 +231,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -558,9 +566,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="63.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -570,11 +578,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -582,7 +590,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
         <v>103</v>
@@ -597,10 +605,10 @@
     </row>
     <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>132.72999999999999</v>
@@ -613,72 +621,72 @@
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
+      <c r="A7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>